<commit_message>
Automation Script for Jira Ticket Creation.
</commit_message>
<xml_diff>
--- a/MavenJira/Excel/Annual Salary Details.xlsx
+++ b/MavenJira/Excel/Annual Salary Details.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{36B4A8A0-BEDD-44C3-A8D5-2AF4436EFAEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0871515C-594B-45FE-BC85-4E92E832C3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23304" windowHeight="13224" activeTab="1" xr2:uid="{D6A124A6-D158-4CEF-9E88-76522D908153}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="23304" windowHeight="13224" activeTab="1" xr2:uid="{D6A124A6-D158-4CEF-9E88-76522D908153}"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
-    <sheet name="RequestID" sheetId="2" r:id="rId2"/>
+    <sheet name="Incident" sheetId="2" r:id="rId2"/>
+    <sheet name="Workorder" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L15"/>
+  <oleSize ref="A1:L24"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Username</t>
   </si>
@@ -45,17 +46,20 @@
     <t>Workorder</t>
   </si>
   <si>
-    <t>INC623846</t>
-  </si>
-  <si>
-    <t>INC623940</t>
+    <t>WO240627</t>
+  </si>
+  <si>
+    <t>WO240628</t>
+  </si>
+  <si>
+    <t>INC789654</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +83,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -94,7 +104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,16 +127,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -491,10 +514,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23DED5A-6031-4F14-BB2C-292D4100DBD3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,25 +527,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2597B8-0EBB-4745-BC0B-879F3A3D018A}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>